<commit_message>
excel to two dim array main method
</commit_message>
<xml_diff>
--- a/test-data/orange_data.xlsx
+++ b/test-data/orange_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mine\Company\MicroFocus2\automation_workspace\OrangeAutomation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,28 +30,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Expected Error</t>
+  </si>
+  <si>
+    <t>bala123</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>kim</t>
+  </si>
+  <si>
+    <t>kim123</t>
+  </si>
+  <si>
     <t>Username</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Expected Error</t>
-  </si>
-  <si>
     <t>bala</t>
-  </si>
-  <si>
-    <t>bala123</t>
-  </si>
-  <si>
-    <t>Invalid credentials</t>
-  </si>
-  <si>
-    <t>kim</t>
-  </si>
-  <si>
-    <t>kim123</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,35 +384,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LoginTest data from excel
</commit_message>
<xml_diff>
--- a/test-data/orange_data.xlsx
+++ b/test-data/orange_data.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invalidLoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="validLoginTest" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="testDemo" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Password</t>
   </si>
@@ -46,16 +46,42 @@
   </si>
   <si>
     <t>saukl</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>ExpectedUrl</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/web/index.php/pim/viewEmployeeList</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +104,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -365,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -405,24 +434,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>454</v>
+      </c>
+      <c r="B2">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>454</v>
+      </c>
+      <c r="B3">
+        <v>554</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
extent report updaed in base class
</commit_message>
<xml_diff>
--- a/test-data/orange_data.xlsx
+++ b/test-data/orange_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="invalidLoginTest" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Password</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>Invalid credentials222</t>
+  </si>
+  <si>
+    <t>saukl222</t>
   </si>
 </sst>
 </file>
@@ -392,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,6 +433,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -436,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>